<commit_message>
nearest neighbour solver, no interval or fixed pos
</commit_message>
<xml_diff>
--- a/Cleansed Show Data.xlsx
+++ b/Cleansed Show Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miran\Documents\CodeStuff\Running Order Wizard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miran\Documents\CodeStuff\Stage Manager\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>SD - Ana Solo</t>
   </si>
@@ -56,9 +56,6 @@
     <t>SD - Josh and Tiggy Duet</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Style</t>
   </si>
   <si>
@@ -249,6 +246,12 @@
   </si>
   <si>
     <t>Person AF</t>
+  </si>
+  <si>
+    <t>Cateogry</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ1008"/>
+  <dimension ref="A1:AJ1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,256 +677,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="B1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="AJ1" s="4"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="6">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1</v>
+      </c>
+      <c r="I2" s="6">
+        <v>1</v>
+      </c>
+      <c r="J2" s="6">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>1</v>
+      </c>
+      <c r="L2" s="6">
+        <v>1</v>
+      </c>
+      <c r="M2" s="6">
+        <v>1</v>
+      </c>
+      <c r="N2" s="6">
+        <v>1</v>
+      </c>
+      <c r="O2" s="6">
+        <v>1</v>
+      </c>
+      <c r="P2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>1</v>
+      </c>
+      <c r="R2" s="6">
+        <v>1</v>
+      </c>
+      <c r="S2" s="6">
+        <v>1</v>
+      </c>
+      <c r="T2" s="6">
+        <v>1</v>
+      </c>
+      <c r="U2" s="6">
+        <v>1</v>
+      </c>
+      <c r="V2" s="6">
+        <v>1</v>
+      </c>
+      <c r="W2" s="6">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="7"/>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AI1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="AJ1" s="4"/>
-    </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="AJ2" s="7"/>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="E3" s="6">
-        <v>1</v>
-      </c>
-      <c r="F3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3" s="6">
-        <v>1</v>
-      </c>
-      <c r="H3" s="6">
-        <v>1</v>
-      </c>
-      <c r="I3" s="6">
-        <v>1</v>
-      </c>
-      <c r="J3" s="6">
-        <v>1</v>
-      </c>
-      <c r="K3" s="6">
-        <v>1</v>
-      </c>
-      <c r="L3" s="6">
-        <v>1</v>
-      </c>
-      <c r="M3" s="6">
-        <v>1</v>
-      </c>
-      <c r="N3" s="6">
-        <v>1</v>
-      </c>
-      <c r="O3" s="6">
-        <v>1</v>
-      </c>
-      <c r="P3" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="6">
-        <v>1</v>
-      </c>
-      <c r="R3" s="6">
-        <v>1</v>
-      </c>
-      <c r="S3" s="6">
-        <v>1</v>
-      </c>
-      <c r="T3" s="6">
-        <v>1</v>
-      </c>
-      <c r="U3" s="6">
-        <v>1</v>
-      </c>
-      <c r="V3" s="6">
-        <v>1</v>
-      </c>
-      <c r="W3" s="6">
-        <v>1</v>
-      </c>
-      <c r="X3" s="6">
-        <v>1</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>1</v>
-      </c>
-      <c r="Z3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="6">
+      <c r="B3" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>1</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1</v>
+      </c>
+      <c r="R3" s="9">
+        <v>1</v>
+      </c>
+      <c r="T3" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="9">
         <v>1</v>
       </c>
       <c r="AJ3" s="7"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="9">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="9">
-        <v>1</v>
-      </c>
-      <c r="I4" s="9">
-        <v>1</v>
-      </c>
       <c r="J4" s="9">
         <v>1</v>
       </c>
+      <c r="K4" s="9">
+        <v>1</v>
+      </c>
+      <c r="L4" s="9">
+        <v>1</v>
+      </c>
+      <c r="M4" s="9">
+        <v>1</v>
+      </c>
       <c r="N4" s="9">
         <v>1</v>
       </c>
+      <c r="O4" s="9">
+        <v>1</v>
+      </c>
       <c r="R4" s="9">
         <v>1</v>
       </c>
+      <c r="S4" s="9">
+        <v>1</v>
+      </c>
       <c r="T4" s="9">
         <v>1</v>
       </c>
-      <c r="Y4" s="9">
+      <c r="U4" s="9">
+        <v>1</v>
+      </c>
+      <c r="W4" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="9">
         <v>1</v>
       </c>
       <c r="AA4" s="9">
@@ -932,46 +1001,34 @@
       <c r="AB4" s="9">
         <v>1</v>
       </c>
-      <c r="AF4" s="9">
-        <v>1</v>
-      </c>
       <c r="AG4" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="9">
         <v>1</v>
       </c>
       <c r="AJ4" s="7"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="9">
+        <v>21</v>
+      </c>
+      <c r="D5" s="9">
         <v>1</v>
       </c>
       <c r="J5" s="9">
         <v>1</v>
       </c>
-      <c r="K5" s="9">
-        <v>1</v>
-      </c>
-      <c r="L5" s="9">
-        <v>1</v>
-      </c>
       <c r="M5" s="9">
         <v>1</v>
       </c>
-      <c r="N5" s="9">
-        <v>1</v>
-      </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="9">
         <v>1</v>
       </c>
       <c r="R5" s="9">
@@ -983,22 +1040,25 @@
       <c r="T5" s="9">
         <v>1</v>
       </c>
-      <c r="U5" s="9">
-        <v>1</v>
-      </c>
-      <c r="W5" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="9">
+      <c r="V5" s="9">
+        <v>1</v>
+      </c>
+      <c r="X5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="9">
         <v>1</v>
       </c>
       <c r="AG5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH5" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI5" s="9">
         <v>1</v>
       </c>
       <c r="AJ5" s="7"/>
@@ -1008,44 +1068,47 @@
         <v>20</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="J6" s="9">
-        <v>1</v>
-      </c>
-      <c r="M6" s="9">
-        <v>1</v>
-      </c>
-      <c r="P6" s="9">
+      <c r="E6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6" s="9">
         <v>1</v>
       </c>
       <c r="Q6" s="9">
         <v>1</v>
       </c>
-      <c r="R6" s="9">
-        <v>1</v>
-      </c>
       <c r="S6" s="9">
         <v>1</v>
       </c>
-      <c r="T6" s="9">
-        <v>1</v>
-      </c>
-      <c r="V6" s="9">
+      <c r="U6" s="9">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9">
         <v>1</v>
       </c>
       <c r="X6" s="9">
         <v>1</v>
       </c>
+      <c r="Z6" s="9">
+        <v>1</v>
+      </c>
       <c r="AC6" s="9">
         <v>1</v>
       </c>
+      <c r="AD6" s="9">
+        <v>1</v>
+      </c>
       <c r="AE6" s="9">
         <v>1</v>
       </c>
@@ -1053,130 +1116,130 @@
         <v>1</v>
       </c>
       <c r="AH6" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="9">
         <v>1</v>
       </c>
       <c r="AJ6" s="7"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="9">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9">
+        <v>23</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1</v>
+      </c>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1</v>
+      </c>
+      <c r="K7" s="9">
+        <v>1</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1</v>
+      </c>
+      <c r="N7" s="9">
         <v>1</v>
       </c>
       <c r="O7" s="9">
         <v>1</v>
       </c>
-      <c r="Q7" s="9">
-        <v>1</v>
-      </c>
       <c r="S7" s="9">
         <v>1</v>
       </c>
-      <c r="U7" s="9">
-        <v>1</v>
-      </c>
-      <c r="W7" s="9">
-        <v>1</v>
-      </c>
-      <c r="X7" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AD7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AE7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AG7" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH7" s="9">
+      <c r="T7" s="9">
+        <v>1</v>
+      </c>
+      <c r="V7" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI7" s="9">
         <v>1</v>
       </c>
       <c r="AJ7" s="7"/>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>24</v>
+      <c r="E8" s="9">
+        <v>1</v>
       </c>
       <c r="F8" s="9">
         <v>1</v>
       </c>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="I8" s="9">
-        <v>1</v>
-      </c>
       <c r="K8" s="9">
         <v>1</v>
       </c>
-      <c r="L8" s="9">
-        <v>1</v>
-      </c>
-      <c r="N8" s="9">
-        <v>1</v>
-      </c>
-      <c r="O8" s="9">
+      <c r="M8" s="9">
+        <v>1</v>
+      </c>
+      <c r="P8" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>1</v>
+      </c>
+      <c r="R8" s="9">
         <v>1</v>
       </c>
       <c r="S8" s="9">
         <v>1</v>
       </c>
-      <c r="T8" s="9">
-        <v>1</v>
-      </c>
-      <c r="V8" s="9">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AF8" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI8" s="9">
+      <c r="U8" s="9">
+        <v>1</v>
+      </c>
+      <c r="W8" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG8" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="9">
         <v>1</v>
       </c>
       <c r="AJ8" s="7"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="E9" s="9">
         <v>1</v>
@@ -1184,82 +1247,82 @@
       <c r="F9" s="9">
         <v>1</v>
       </c>
-      <c r="K9" s="9">
-        <v>1</v>
-      </c>
-      <c r="M9" s="9">
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="9">
         <v>1</v>
       </c>
       <c r="P9" s="9">
         <v>1</v>
       </c>
-      <c r="Q9" s="9">
-        <v>1</v>
-      </c>
-      <c r="R9" s="9">
-        <v>1</v>
-      </c>
-      <c r="S9" s="9">
-        <v>1</v>
-      </c>
-      <c r="U9" s="9">
-        <v>1</v>
-      </c>
       <c r="W9" s="9">
         <v>1</v>
       </c>
       <c r="Z9" s="9">
         <v>1</v>
       </c>
-      <c r="AA9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AG9" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="9">
+      <c r="AD9" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="9">
         <v>1</v>
       </c>
       <c r="AJ9" s="7"/>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9">
-        <v>1</v>
-      </c>
-      <c r="L10" s="9">
+        <v>27</v>
+      </c>
+      <c r="J10" s="9">
+        <v>1</v>
+      </c>
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+      <c r="M10" s="9">
+        <v>1</v>
+      </c>
+      <c r="O10" s="9">
         <v>1</v>
       </c>
       <c r="P10" s="9">
         <v>1</v>
       </c>
+      <c r="Q10" s="10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="9">
+        <v>1</v>
+      </c>
+      <c r="S10" s="9">
+        <v>1</v>
+      </c>
+      <c r="V10" s="9">
+        <v>1</v>
+      </c>
       <c r="W10" s="9">
         <v>1</v>
       </c>
-      <c r="Z10" s="9">
+      <c r="X10" s="9">
         <v>1</v>
       </c>
       <c r="AD10" s="9">
+        <v>1</v>
+      </c>
+      <c r="AE10" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG10" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="9">
         <v>1</v>
       </c>
       <c r="AI10" s="9">
@@ -1269,90 +1332,72 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J11" s="9">
+        <v>30</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
         <v>1</v>
       </c>
       <c r="K11" s="9">
         <v>1</v>
       </c>
-      <c r="M11" s="9">
-        <v>1</v>
-      </c>
-      <c r="O11" s="9">
-        <v>1</v>
-      </c>
-      <c r="P11" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="10">
-        <v>1</v>
-      </c>
-      <c r="R11" s="9">
-        <v>1</v>
-      </c>
-      <c r="S11" s="9">
-        <v>1</v>
-      </c>
-      <c r="V11" s="9">
-        <v>1</v>
-      </c>
-      <c r="W11" s="9">
-        <v>1</v>
-      </c>
-      <c r="X11" s="9">
+      <c r="N11" s="9">
         <v>1</v>
       </c>
       <c r="AD11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AE11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI11" s="9">
         <v>1</v>
       </c>
       <c r="AJ11" s="7"/>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9">
+        <v>21</v>
+      </c>
+      <c r="J12" s="9">
         <v>1</v>
       </c>
       <c r="K12" s="9">
         <v>1</v>
       </c>
-      <c r="N12" s="9">
-        <v>1</v>
-      </c>
-      <c r="AD12" s="9">
+      <c r="P12" s="9">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>1</v>
+      </c>
+      <c r="R12" s="9">
+        <v>1</v>
+      </c>
+      <c r="S12" s="9">
+        <v>1</v>
+      </c>
+      <c r="T12" s="9">
+        <v>1</v>
+      </c>
+      <c r="V12" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="9">
         <v>1</v>
       </c>
       <c r="AJ12" s="7"/>
@@ -1362,66 +1407,54 @@
         <v>32</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="9">
-        <v>1</v>
-      </c>
-      <c r="K13" s="9">
-        <v>1</v>
-      </c>
-      <c r="P13" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="9">
-        <v>1</v>
-      </c>
-      <c r="R13" s="9">
-        <v>1</v>
-      </c>
-      <c r="S13" s="9">
-        <v>1</v>
-      </c>
-      <c r="T13" s="9">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="V13" s="9">
         <v>1</v>
       </c>
-      <c r="AA13" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="9">
+      <c r="Y13" s="9">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="9">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI13" s="9">
         <v>1</v>
       </c>
       <c r="AJ13" s="7"/>
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="V14" s="9">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="9">
+        <v>27</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1</v>
+      </c>
+      <c r="M14" s="9">
+        <v>1</v>
+      </c>
+      <c r="W14" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="9">
         <v>1</v>
       </c>
       <c r="AB14" s="9">
         <v>1</v>
       </c>
       <c r="AF14" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI14" s="9">
         <v>1</v>
       </c>
       <c r="AJ14" s="7"/>
@@ -1431,27 +1464,42 @@
         <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="K15" s="9">
+        <v>16</v>
+      </c>
+      <c r="L15" s="9">
         <v>1</v>
       </c>
       <c r="M15" s="9">
         <v>1</v>
       </c>
-      <c r="W15" s="9">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="9">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="9">
-        <v>1</v>
-      </c>
-      <c r="AF15" s="9">
+      <c r="Q15" s="9">
+        <v>1</v>
+      </c>
+      <c r="S15" s="9">
+        <v>1</v>
+      </c>
+      <c r="T15" s="9">
+        <v>1</v>
+      </c>
+      <c r="X15" s="9">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="9">
+        <v>1</v>
+      </c>
+      <c r="AD15" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="9">
         <v>1</v>
       </c>
       <c r="AJ15" s="7"/>
@@ -1461,27 +1509,24 @@
         <v>36</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L16" s="9">
-        <v>1</v>
-      </c>
-      <c r="M16" s="9">
+        <v>27</v>
+      </c>
+      <c r="J16" s="9">
+        <v>1</v>
+      </c>
+      <c r="P16" s="9">
         <v>1</v>
       </c>
       <c r="Q16" s="9">
         <v>1</v>
       </c>
-      <c r="S16" s="9">
-        <v>1</v>
-      </c>
-      <c r="T16" s="9">
-        <v>1</v>
-      </c>
-      <c r="X16" s="9">
+      <c r="U16" s="9">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="9">
         <v>1</v>
       </c>
       <c r="AA16" s="9">
@@ -1494,6 +1539,9 @@
         <v>1</v>
       </c>
       <c r="AG16" s="9">
+        <v>1</v>
+      </c>
+      <c r="AH16" s="9">
         <v>1</v>
       </c>
       <c r="AI16" s="9">
@@ -1506,15 +1554,12 @@
         <v>37</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J17" s="9">
-        <v>1</v>
-      </c>
-      <c r="P17" s="9">
+        <v>21</v>
+      </c>
+      <c r="D17" s="9">
         <v>1</v>
       </c>
       <c r="Q17" s="9">
@@ -1523,25 +1568,16 @@
       <c r="U17" s="9">
         <v>1</v>
       </c>
-      <c r="Z17" s="9">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="9">
+      <c r="X17" s="9">
         <v>1</v>
       </c>
       <c r="AC17" s="9">
         <v>1</v>
       </c>
-      <c r="AD17" s="9">
-        <v>1</v>
-      </c>
-      <c r="AG17" s="9">
+      <c r="AF17" s="9">
         <v>1</v>
       </c>
       <c r="AH17" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI17" s="9">
         <v>1</v>
       </c>
       <c r="AJ17" s="7"/>
@@ -1551,30 +1587,21 @@
         <v>38</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="9">
-        <v>1</v>
-      </c>
-      <c r="U18" s="9">
-        <v>1</v>
-      </c>
-      <c r="X18" s="9">
-        <v>1</v>
-      </c>
-      <c r="AC18" s="9">
-        <v>1</v>
-      </c>
-      <c r="AF18" s="9">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="9">
+      <c r="I18" s="9">
+        <v>1</v>
+      </c>
+      <c r="N18" s="9">
+        <v>1</v>
+      </c>
+      <c r="P18" s="9">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="9">
         <v>1</v>
       </c>
       <c r="AJ18" s="7"/>
@@ -1584,302 +1611,281 @@
         <v>39</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="I19" s="9">
+        <v>18</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="L19" s="9">
         <v>1</v>
       </c>
       <c r="N19" s="9">
         <v>1</v>
       </c>
-      <c r="P19" s="9">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="9">
+      <c r="O19" s="9">
+        <v>1</v>
+      </c>
+      <c r="V19" s="9">
+        <v>1</v>
+      </c>
+      <c r="W19" s="9">
+        <v>1</v>
+      </c>
+      <c r="AI19" s="9">
         <v>1</v>
       </c>
       <c r="AJ19" s="7"/>
     </row>
     <row r="20" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>30</v>
-      </c>
       <c r="C20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="9"/>
-      <c r="L20" s="9">
-        <v>1</v>
-      </c>
-      <c r="N20" s="9">
-        <v>1</v>
-      </c>
-      <c r="O20" s="9">
-        <v>1</v>
-      </c>
-      <c r="V20" s="9">
-        <v>1</v>
-      </c>
-      <c r="W20" s="9">
-        <v>1</v>
-      </c>
-      <c r="AI20" s="9">
+        <v>13</v>
+      </c>
+      <c r="G20" s="9">
         <v>1</v>
       </c>
       <c r="AJ20" s="7"/>
     </row>
     <row r="21" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="9">
+        <v>25</v>
+      </c>
+      <c r="H21" s="9">
         <v>1</v>
       </c>
       <c r="AJ21" s="7"/>
     </row>
     <row r="22" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" s="9">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="N22" s="9">
+        <v>1</v>
+      </c>
+      <c r="O22" s="9"/>
       <c r="AJ22" s="7"/>
     </row>
     <row r="23" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="N23" s="9">
-        <v>1</v>
-      </c>
-      <c r="O23" s="9"/>
+        <v>18</v>
+      </c>
+      <c r="O23" s="9">
+        <v>1</v>
+      </c>
       <c r="AJ23" s="7"/>
     </row>
     <row r="24" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O24" s="9">
+        <v>21</v>
+      </c>
+      <c r="X24" s="9">
         <v>1</v>
       </c>
       <c r="AJ24" s="7"/>
     </row>
     <row r="25" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="X25" s="9">
+        <v>18</v>
+      </c>
+      <c r="Z25" s="9">
         <v>1</v>
       </c>
       <c r="AJ25" s="7"/>
     </row>
     <row r="26" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z26" s="9">
+        <v>21</v>
+      </c>
+      <c r="AE26" s="9">
         <v>1</v>
       </c>
       <c r="AJ26" s="7"/>
     </row>
     <row r="27" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE27" s="9">
+        <v>18</v>
+      </c>
+      <c r="AI27" s="9">
         <v>1</v>
       </c>
       <c r="AJ27" s="7"/>
     </row>
     <row r="28" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="AI28" s="9">
+        <v>18</v>
+      </c>
+      <c r="O28" s="9">
+        <v>1</v>
+      </c>
+      <c r="S28" s="9">
         <v>1</v>
       </c>
       <c r="AJ28" s="7"/>
     </row>
     <row r="29" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="O29" s="9">
-        <v>1</v>
-      </c>
-      <c r="S29" s="9">
+        <v>18</v>
+      </c>
+      <c r="W29" s="9">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="9">
         <v>1</v>
       </c>
       <c r="AJ29" s="7"/>
     </row>
     <row r="30" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A30" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="W30" s="9">
-        <v>1</v>
-      </c>
-      <c r="AG30" s="9">
-        <v>1</v>
-      </c>
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
+      <c r="AI30" s="7"/>
       <c r="AJ30" s="7"/>
     </row>
     <row r="31" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AE31" s="9"/>
       <c r="AJ31" s="7"/>
     </row>
     <row r="32" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A32" s="11"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
-      <c r="V32" s="7"/>
-      <c r="W32" s="7"/>
-      <c r="X32" s="7"/>
-      <c r="Y32" s="7"/>
-      <c r="Z32" s="7"/>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="7"/>
-      <c r="AD32" s="7"/>
-      <c r="AE32" s="7"/>
-      <c r="AF32" s="7"/>
-      <c r="AG32" s="7"/>
-      <c r="AH32" s="7"/>
-      <c r="AI32" s="7"/>
+      <c r="F32" s="12"/>
       <c r="AJ32" s="7"/>
     </row>
-    <row r="33" spans="6:36" x14ac:dyDescent="0.35">
-      <c r="AE33" s="9"/>
+    <row r="33" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ33" s="7"/>
     </row>
-    <row r="34" spans="6:36" x14ac:dyDescent="0.35">
-      <c r="F34" s="12"/>
+    <row r="34" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ34" s="7"/>
     </row>
-    <row r="35" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="35" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ35" s="7"/>
     </row>
-    <row r="36" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="36" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ36" s="7"/>
     </row>
-    <row r="37" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="37" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ37" s="7"/>
     </row>
-    <row r="38" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="38" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ38" s="7"/>
     </row>
-    <row r="39" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="39" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ39" s="7"/>
     </row>
-    <row r="40" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="40" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ40" s="7"/>
     </row>
-    <row r="41" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="41" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ41" s="7"/>
     </row>
-    <row r="42" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="42" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ42" s="7"/>
     </row>
-    <row r="43" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="43" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ43" s="7"/>
     </row>
-    <row r="44" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="44" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ44" s="7"/>
     </row>
-    <row r="45" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="45" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ45" s="7"/>
     </row>
-    <row r="46" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="46" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ46" s="7"/>
     </row>
-    <row r="47" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="47" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ47" s="7"/>
     </row>
-    <row r="48" spans="6:36" x14ac:dyDescent="0.35">
+    <row r="48" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ48" s="7"/>
     </row>
     <row r="49" spans="36:36" x14ac:dyDescent="0.35">
@@ -4755,12 +4761,6 @@
     </row>
     <row r="1006" spans="36:36" x14ac:dyDescent="0.35">
       <c r="AJ1006" s="7"/>
-    </row>
-    <row r="1007" spans="36:36" x14ac:dyDescent="0.35">
-      <c r="AJ1007" s="7"/>
-    </row>
-    <row r="1008" spans="36:36" x14ac:dyDescent="0.35">
-      <c r="AJ1008" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>